<commit_message>
Atualização da planilha, inseri mais 2 exemplos
</commit_message>
<xml_diff>
--- a/Planilha.xlsx
+++ b/Planilha.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19515" windowHeight="8340" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19515" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="Bar" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="34">
   <si>
     <t>Sexo</t>
   </si>
@@ -110,6 +110,18 @@
   </si>
   <si>
     <t>(abatimentos)</t>
+  </si>
+  <si>
+    <t>Exemplo 1</t>
+  </si>
+  <si>
+    <t>Exemplo 2</t>
+  </si>
+  <si>
+    <t>Exemplo 3</t>
+  </si>
+  <si>
+    <t>M</t>
   </si>
 </sst>
 </file>
@@ -117,9 +129,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="_(&quot;R$ &quot;* #,##0.00_);_(&quot;R$ &quot;* \(#,##0.00\);_(&quot;R$ &quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;R$ &quot;* #,##0.00_);_(&quot;R$ &quot;* \(#,##0.00\);_(&quot;R$ &quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -173,6 +185,14 @@
       <color theme="0" tint="-4.9989318521683403E-2"/>
       <name val="Courier New"/>
       <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -244,15 +264,15 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -262,9 +282,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
@@ -538,7 +559,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -546,124 +567,272 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:K13"/>
+  <dimension ref="B1:J13"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="21.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.28515625" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="21.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C2" s="1" t="s">
+    <row r="1" spans="2:10" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B1" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="C2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="1"/>
-      <c r="K2" s="4"/>
-    </row>
-    <row r="3" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C3" s="1" t="s">
+      <c r="E2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="4"/>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="9">
+      <c r="C3" s="9">
+        <v>5</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J3" s="1"/>
-      <c r="K3" s="4"/>
-    </row>
-    <row r="4" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C4" s="1" t="s">
+      <c r="F3" s="9">
+        <v>5</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="9">
+        <v>0</v>
+      </c>
+      <c r="J3" s="4"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="9">
+      <c r="C4" s="9">
         <v>1</v>
       </c>
-      <c r="J4" s="1"/>
-      <c r="K4" s="4"/>
-    </row>
-    <row r="5" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C5" s="1" t="s">
+      <c r="E4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="9">
+        <v>4</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" s="9">
+        <v>1</v>
+      </c>
+      <c r="J4" s="4"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="9">
-        <v>1</v>
-      </c>
-      <c r="J5" s="1"/>
-      <c r="K5" s="4"/>
-    </row>
-    <row r="6" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C6" s="2"/>
-      <c r="D6" s="7"/>
-    </row>
-    <row r="7" spans="3:11" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="C7" s="8" t="s">
+      <c r="C5" s="9">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="9">
+        <v>4</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I5" s="9">
+        <v>3</v>
+      </c>
+      <c r="J5" s="4"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="2"/>
+      <c r="C6" s="7"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="7"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="7"/>
+    </row>
+    <row r="7" spans="2:10" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="6"/>
-    </row>
-    <row r="8" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C8" s="1" t="s">
+      <c r="C7" s="6"/>
+      <c r="E7" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="6"/>
+      <c r="H7" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" s="6"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="14">
-        <f>IF(D2="M",10,IF(D2="","",8))</f>
+      <c r="C8" s="14">
+        <f>IF(C2="M",10,IF(C2="","",8))</f>
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C9" s="1" t="s">
+      <c r="E8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="14">
+        <f>IF(F2="M",10,IF(F2="","",8))</f>
+        <v>10</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8" s="14">
+        <f>IF(I2="M",10,IF(I2="","",8))</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="14">
-        <f>D3*2.5+D4*2+D5*4</f>
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="10" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C10" s="1" t="s">
+      <c r="C9" s="14">
+        <f>C3*2.5+C4*2+C5*4</f>
+        <v>14.5</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="14">
+        <f>F3*2.5+F4*2+F5*4</f>
+        <v>36.5</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I9" s="14">
+        <f>I3*2.5+I4*2+I5*4</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="14">
-        <f>IF(D9&lt;=15,3,0)</f>
+      <c r="C10" s="14">
+        <f>IF(C9&lt;=15,3,0)</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C11" s="1" t="s">
+      <c r="E10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="14">
+        <f>IF(F9&lt;=15,3,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I10" s="14">
+        <f>IF(I9&lt;=15,3,0)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="14">
-        <f>SUM(D8:D10)</f>
-        <v>19.5</v>
-      </c>
-    </row>
-    <row r="12" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C12" s="3" t="s">
+      <c r="C11" s="14">
+        <f>SUM(C8:C10)</f>
+        <v>25.5</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="14">
+        <f>SUM(F8:F10)</f>
+        <v>46.5</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11" s="14">
+        <f>SUM(I8:I10)</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="5"/>
-    </row>
-    <row r="13" spans="3:11" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="C13" s="11" t="s">
+      <c r="C12" s="5"/>
+      <c r="E12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="5"/>
+      <c r="H12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I12" s="5"/>
+    </row>
+    <row r="13" spans="2:10" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B13" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="14">
-        <f>D11*110%</f>
-        <v>21.450000000000003</v>
+      <c r="C13" s="14">
+        <f>C11*110%</f>
+        <v>28.05</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="14">
+        <f>F11*110%</f>
+        <v>51.150000000000006</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I13" s="14">
+        <f>I11*110%</f>
+        <v>29.700000000000003</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2 F2 I2">
       <formula1>"M,F"</formula1>
     </dataValidation>
   </dataValidations>
@@ -674,196 +843,481 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:E25"/>
+  <dimension ref="B2:L25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="20.42578125" customWidth="1"/>
-    <col min="4" max="4" width="34.85546875" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" customWidth="1"/>
+    <col min="3" max="3" width="34.85546875" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" customWidth="1"/>
+    <col min="7" max="7" width="34.85546875" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" customWidth="1"/>
+    <col min="10" max="10" width="20.42578125" customWidth="1"/>
+    <col min="11" max="11" width="34.85546875" customWidth="1"/>
+    <col min="12" max="12" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C3" s="1" t="s">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B2" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" s="16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="13">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C4" s="1" t="s">
+      <c r="D3" s="13">
+        <v>5000</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="13">
+        <v>30000</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" s="13">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="13">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C5" s="1" t="s">
+      <c r="D4" s="13">
+        <v>4880</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="13">
+        <v>5487.03</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L4" s="13">
+        <v>3487.47</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="13">
+      <c r="D5" s="13">
         <v>1500</v>
       </c>
-    </row>
-    <row r="6" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C6" s="1" t="s">
+      <c r="F5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="13">
+        <v>2400</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L5" s="13">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="13">
+      <c r="D6" s="13">
         <v>400</v>
       </c>
-    </row>
-    <row r="7" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C7" s="1" t="s">
+      <c r="F6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="13">
+        <v>400</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L6" s="13">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="13">
+      <c r="D7" s="13">
         <v>2400</v>
       </c>
-    </row>
-    <row r="8" spans="3:5" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="C8" s="11" t="s">
+      <c r="F7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="13">
+        <v>500</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L7" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B8" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="12"/>
-    </row>
-    <row r="9" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C9" s="14">
-        <f>20%*E3</f>
+      <c r="C8" s="10"/>
+      <c r="D8" s="12"/>
+      <c r="F8" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="10"/>
+      <c r="H8" s="12"/>
+      <c r="J8" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" s="10"/>
+      <c r="L8" s="12"/>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B9" s="14">
+        <f>20%*D3</f>
+        <v>1000</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="14">
+        <f>20%*H3</f>
+        <v>6000</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J9" s="14">
+        <f>20%*L3</f>
+        <v>100</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B10" s="14">
+        <f>IF(D4&gt;24000,20%,IF(D4&gt;8000,15%,0))*D4</f>
+        <v>0</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="14">
+        <f>IF(H4&gt;24000,20%,IF(H4&gt;8000,15%,0))*H4</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J10" s="14">
+        <f>IF(L4&gt;24000,20%,IF(L4&gt;8000,15%,0))*L4</f>
+        <v>0</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B11" s="15">
+        <f>10%*D5</f>
+        <v>150</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="15">
+        <f>10%*H5</f>
         <v>240</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C10" s="14">
-        <f>IF(E4&gt;24000,20%,IF(E4&gt;8000,15%,0))*E4</f>
-        <v>3000</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="3:5" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="C11" s="15">
-        <f>10%*E5</f>
-        <v>150</v>
-      </c>
-      <c r="D11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="12" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C12" s="14">
-        <f>SUM(C9:C11)</f>
-        <v>3390</v>
-      </c>
-      <c r="D12" s="1" t="s">
+      <c r="J11" s="15">
+        <f>10%*L5</f>
+        <v>40</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="14">
+        <f>SUM(B9:B11)</f>
+        <v>1150</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="13" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C13" s="1" t="s">
+      <c r="F12" s="14">
+        <f>SUM(F9:F11)</f>
+        <v>6240</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J12" s="14">
+        <f>SUM(J9:J11)</f>
+        <v>140</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C14" s="1" t="s">
+      <c r="C13" s="1"/>
+      <c r="F13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="1"/>
+      <c r="J13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C15" s="14">
-        <f>C12*30%</f>
-        <v>1017</v>
-      </c>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C16" s="1" t="s">
+      <c r="C14" s="1"/>
+      <c r="F14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" s="1"/>
+      <c r="J14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K14" s="1"/>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B15" s="14">
+        <f>B12*30%</f>
+        <v>345</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="F15" s="14">
+        <f>F12*30%</f>
+        <v>1872</v>
+      </c>
+      <c r="G15" s="1"/>
+      <c r="J15" s="14">
+        <f>J12*30%</f>
+        <v>42</v>
+      </c>
+      <c r="K15" s="1"/>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C17" s="1" t="s">
+      <c r="C16" s="1"/>
+      <c r="F16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="1"/>
+      <c r="J16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K16" s="1"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C18" s="14">
-        <f>E6</f>
+      <c r="C17" s="1"/>
+      <c r="F17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" s="1"/>
+      <c r="J17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K17" s="1"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="14">
+        <f>D6</f>
         <v>400</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C19" s="14">
-        <f>E7</f>
+      <c r="F18" s="14">
+        <f>H6</f>
+        <v>400</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J18" s="14">
+        <f>L6</f>
+        <v>874</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="14">
+        <f>D7</f>
         <v>2400</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C20" s="14">
-        <f>SUM(C18:C19)</f>
+      <c r="F19" s="14">
+        <f>H7</f>
+        <v>500</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J19" s="14">
+        <f>L7</f>
+        <v>0</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="14">
+        <f>SUM(B18:B19)</f>
         <v>2800</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C21" s="1" t="s">
+      <c r="F20" s="14">
+        <f>SUM(F18:F19)</f>
+        <v>900</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J20" s="14">
+        <f>SUM(J18:J19)</f>
+        <v>874</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C22" s="1" t="s">
+      <c r="C21" s="1"/>
+      <c r="F21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="1"/>
+      <c r="J21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K21" s="1"/>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C23" s="14">
-        <f>C12</f>
-        <v>3390</v>
-      </c>
-      <c r="D23" s="1" t="s">
+      <c r="C22" s="1"/>
+      <c r="F22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" s="1"/>
+      <c r="J22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K22" s="1"/>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B23" s="14">
+        <f>B12</f>
+        <v>1150</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C24" s="14">
-        <f>IF(SUM(C18:C20)&gt;C15,C15,C15)</f>
-        <v>1017</v>
-      </c>
-      <c r="D24" s="1" t="s">
+      <c r="F23" s="14">
+        <f>F12</f>
+        <v>6240</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J23" s="14">
+        <f>J12</f>
+        <v>140</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B24" s="14">
+        <f>IF(SUM(B18:B20)&gt;B15,B15,B15)</f>
+        <v>345</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="25" spans="3:4" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="C25" s="14">
-        <f>C23-C24</f>
-        <v>2373</v>
-      </c>
-      <c r="D25" s="11" t="s">
+      <c r="F24" s="14">
+        <f>IF(SUM(F18:F20)&gt;F15,F15,F15)</f>
+        <v>1872</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J24" s="14">
+        <f>IF(SUM(J18:J20)&gt;J15,J15,J15)</f>
+        <v>42</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B25" s="14">
+        <f>B23-B24</f>
+        <v>805</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F25" s="14">
+        <f>F23-F24</f>
+        <v>4368</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="J25" s="14">
+        <f>J23-J24</f>
+        <v>98</v>
+      </c>
+      <c r="K25" s="11" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>